<commit_message>
type: feat Release the restrictions
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/detailed_results.xlsx
+++ b/POS Code/Experiments/attachments/detailed_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7923D620-256F-BE4C-8B81-8E5F909D1D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA55F03C-0BCB-4B80-811E-1DAD684B6DD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="2740" windowWidth="27540" windowHeight="17700" activeTab="2" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
+    <workbookView xWindow="5520" yWindow="2745" windowWidth="27540" windowHeight="17700" activeTab="2" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="POSSummary" sheetId="3" r:id="rId1"/>
@@ -221,7 +221,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -425,23 +425,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -472,6 +457,24 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -23983,28 +23986,28 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -24046,8 +24049,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -24090,8 +24093,8 @@
         <v>9984</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
+    <row r="3" spans="1:14">
+      <c r="A3" s="41"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -24132,8 +24135,8 @@
         <v>0.96009999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" s="39" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -24176,8 +24179,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
+    <row r="5" spans="1:14">
+      <c r="A5" s="41"/>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -24218,8 +24221,8 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:14">
+      <c r="A6" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -24262,8 +24265,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
+    <row r="7" spans="1:14">
+      <c r="A7" s="40"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -24304,8 +24307,8 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
+    <row r="8" spans="1:14">
+      <c r="A8" s="40"/>
       <c r="B8" s="26" t="s">
         <v>41</v>
       </c>
@@ -24358,8 +24361,8 @@
         <v>-1.6100000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
+    <row r="9" spans="1:14">
+      <c r="A9" s="41"/>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -24400,8 +24403,8 @@
         <v>0.99609999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:14">
+      <c r="A10" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -24444,8 +24447,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
+    <row r="11" spans="1:14">
+      <c r="A11" s="40"/>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -24486,8 +24489,8 @@
         <v>0.96309999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
+    <row r="12" spans="1:14">
+      <c r="A12" s="40"/>
       <c r="B12" s="26" t="s">
         <v>41</v>
       </c>
@@ -24540,8 +24543,8 @@
         <v>3.0000000000000027E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
+    <row r="13" spans="1:14">
+      <c r="A13" s="41"/>
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
@@ -24582,8 +24585,8 @@
         <v>0.98309999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -24626,8 +24629,8 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
+    <row r="15" spans="1:14">
+      <c r="A15" s="40"/>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -24668,8 +24671,8 @@
         <v>3406</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
+    <row r="16" spans="1:14">
+      <c r="A16" s="40"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -24710,8 +24713,8 @@
         <v>0.99029999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:14">
+      <c r="A17" s="40"/>
       <c r="B17" s="26" t="s">
         <v>41</v>
       </c>
@@ -24764,8 +24767,8 @@
         <v>3.0200000000000005E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
+    <row r="18" spans="1:14">
+      <c r="A18" s="41"/>
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
@@ -24807,8 +24810,8 @@
         <v>0.65890000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
+    <row r="19" spans="1:14">
+      <c r="A19" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -24851,8 +24854,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:14">
+      <c r="A20" s="40"/>
       <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
@@ -24893,8 +24896,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:14">
+      <c r="A21" s="40"/>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
@@ -24935,8 +24938,8 @@
         <v>768</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:14">
+      <c r="A22" s="40"/>
       <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
@@ -24977,8 +24980,8 @@
         <v>0.99329999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:14">
+      <c r="A23" s="40"/>
       <c r="B23" s="26" t="s">
         <v>41</v>
       </c>
@@ -25031,8 +25034,8 @@
         <v>3.3200000000000007E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:14">
+      <c r="A24" s="41"/>
       <c r="B24" s="4" t="s">
         <v>7</v>
       </c>
@@ -25073,8 +25076,8 @@
         <v>0.92310000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:14">
+      <c r="A25" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -25117,8 +25120,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="31"/>
+    <row r="26" spans="1:14">
+      <c r="A26" s="40"/>
       <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
@@ -25159,8 +25162,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="31"/>
+    <row r="27" spans="1:14">
+      <c r="A27" s="40"/>
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
@@ -25201,8 +25204,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
+    <row r="28" spans="1:14">
+      <c r="A28" s="40"/>
       <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
@@ -25243,8 +25246,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
+    <row r="29" spans="1:14">
+      <c r="A29" s="40"/>
       <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
@@ -25285,8 +25288,8 @@
         <v>0.99029999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="31"/>
+    <row r="30" spans="1:14">
+      <c r="A30" s="40"/>
       <c r="B30" s="26" t="s">
         <v>41</v>
       </c>
@@ -25339,8 +25342,8 @@
         <v>3.0200000000000005E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="32"/>
+    <row r="31" spans="1:14">
+      <c r="A31" s="41"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
@@ -25404,23 +25407,23 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -25456,8 +25459,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -25494,8 +25497,8 @@
         <v>9984</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
+    <row r="3" spans="1:12">
+      <c r="A3" s="41"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -25530,8 +25533,8 @@
         <v>0.66800000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -25568,8 +25571,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
+    <row r="5" spans="1:12">
+      <c r="A5" s="40"/>
       <c r="B5" s="25" t="s">
         <v>5</v>
       </c>
@@ -25604,8 +25607,8 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
+    <row r="6" spans="1:12">
+      <c r="A6" s="40"/>
       <c r="B6" s="25" t="s">
         <v>41</v>
       </c>
@@ -25650,8 +25653,8 @@
         <v>-1.5000000000000013E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
+    <row r="7" spans="1:12">
+      <c r="A7" s="41"/>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -25696,8 +25699,8 @@
         <v>0.99709535256410253</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -25734,8 +25737,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
+    <row r="9" spans="1:12">
+      <c r="A9" s="40"/>
       <c r="B9" s="25" t="s">
         <v>4</v>
       </c>
@@ -25770,8 +25773,8 @@
         <v>8890</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
+    <row r="10" spans="1:12">
+      <c r="A10" s="40"/>
       <c r="B10" s="25" t="s">
         <v>5</v>
       </c>
@@ -25806,8 +25809,8 @@
         <v>0.67020000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
+    <row r="11" spans="1:12">
+      <c r="A11" s="40"/>
       <c r="B11" s="25" t="s">
         <v>41</v>
       </c>
@@ -25852,8 +25855,8 @@
         <v>2.1999999999999797E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
+    <row r="12" spans="1:12">
+      <c r="A12" s="41"/>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
@@ -25898,8 +25901,8 @@
         <v>0.10957532051282048</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+    <row r="13" spans="1:12">
+      <c r="A13" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -25936,8 +25939,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
+    <row r="14" spans="1:12">
+      <c r="A14" s="40"/>
       <c r="B14" s="25" t="s">
         <v>12</v>
       </c>
@@ -25972,8 +25975,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
+    <row r="15" spans="1:12">
+      <c r="A15" s="40"/>
       <c r="B15" s="25" t="s">
         <v>4</v>
       </c>
@@ -26014,8 +26017,8 @@
         <v>9984</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
+    <row r="16" spans="1:12">
+      <c r="A16" s="40"/>
       <c r="B16" s="25" t="s">
         <v>5</v>
       </c>
@@ -26050,8 +26053,8 @@
         <v>0.73650000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
+    <row r="17" spans="1:12">
+      <c r="A17" s="40"/>
       <c r="B17" s="25" t="s">
         <v>41</v>
       </c>
@@ -26096,8 +26099,8 @@
         <v>6.8500000000000005E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
+    <row r="18" spans="1:12">
+      <c r="A18" s="41"/>
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
@@ -26142,8 +26145,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+    <row r="19" spans="1:12">
+      <c r="A19" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -26180,8 +26183,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:12">
+      <c r="A20" s="40"/>
       <c r="B20" s="25" t="s">
         <v>13</v>
       </c>
@@ -26216,8 +26219,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:12">
+      <c r="A21" s="40"/>
       <c r="B21" s="25" t="s">
         <v>9</v>
       </c>
@@ -26252,8 +26255,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:12">
+      <c r="A22" s="40"/>
       <c r="B22" s="25" t="s">
         <v>4</v>
       </c>
@@ -26288,8 +26291,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:12">
+      <c r="A23" s="40"/>
       <c r="B23" s="25" t="s">
         <v>5</v>
       </c>
@@ -26324,8 +26327,8 @@
         <v>0.65559999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
+    <row r="24" spans="1:12">
+      <c r="A24" s="40"/>
       <c r="B24" s="25" t="s">
         <v>41</v>
       </c>
@@ -26370,8 +26373,8 @@
         <v>-1.2400000000000078E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="32"/>
+    <row r="25" spans="1:12">
+      <c r="A25" s="41"/>
       <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
@@ -26433,58 +26436,58 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -26527,28 +26530,28 @@
         <v>9984</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
+    <row r="3" spans="1:14">
+      <c r="A3" s="41"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="34">
         <v>0.72</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="40"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="35"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -26569,53 +26572,53 @@
       <c r="M4" s="2"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="28" t="s">
+    <row r="5" spans="1:14">
+      <c r="A5" s="40"/>
+      <c r="B5" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="30">
         <v>0.71540000000000004</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="38"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="33"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="28" t="s">
+    <row r="6" spans="1:14">
+      <c r="A6" s="40"/>
+      <c r="B6" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="30">
         <f>C5-C3</f>
         <v>-4.5999999999999375E-3</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="41"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="36"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
+    <row r="7" spans="1:14">
+      <c r="A7" s="41"/>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="37">
         <f>1-C4/C2</f>
         <v>0.98307291666666663</v>
       </c>
@@ -26631,8 +26634,8 @@
       <c r="M7" s="15"/>
       <c r="N7" s="6"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:14">
+      <c r="A8" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -26653,69 +26656,69 @@
       <c r="M8" s="2"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="28" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" s="40"/>
+      <c r="B9" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="16">
         <v>3121</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
-      <c r="B10" s="28" t="s">
+    <row r="10" spans="1:14">
+      <c r="A10" s="40"/>
+      <c r="B10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="31">
         <v>0.73</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="38"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="33"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="28" t="s">
+    <row r="11" spans="1:14">
+      <c r="A11" s="40"/>
+      <c r="B11" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="31">
         <f>C10-C3</f>
         <v>1.0000000000000009E-2</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="38"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="33"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
+    <row r="12" spans="1:14">
+      <c r="A12" s="41"/>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
@@ -26735,14 +26738,14 @@
       <c r="M12" s="5"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="44" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="2"/>
@@ -26757,50 +26760,50 @@
       <c r="M13" s="2"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
-      <c r="B14" s="28" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="40"/>
+      <c r="B14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="29">
         <v>1</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
       <c r="N14" s="11"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
-      <c r="B15" s="28" t="s">
+    <row r="15" spans="1:14">
+      <c r="A15" s="40"/>
+      <c r="B15" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="29">
         <f>13*768</f>
         <v>9984</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
       <c r="N15" s="11"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
-      <c r="B16" s="28" t="s">
+    <row r="16" spans="1:14">
+      <c r="A16" s="40"/>
+      <c r="B16" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="2">
@@ -26818,29 +26821,29 @@
       <c r="M16" s="7"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
-      <c r="B17" s="28" t="s">
+    <row r="17" spans="1:14">
+      <c r="A17" s="40"/>
+      <c r="B17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="31">
         <f>C16-C3</f>
         <v>0</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="38"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="33"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
+    <row r="18" spans="1:14">
+      <c r="A18" s="41"/>
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
@@ -26860,8 +26863,8 @@
       <c r="M18" s="5"/>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+    <row r="19" spans="1:14">
+      <c r="A19" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -26880,9 +26883,9 @@
       <c r="M19" s="2"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
-      <c r="B20" s="28" t="s">
+    <row r="20" spans="1:14">
+      <c r="A20" s="40"/>
+      <c r="B20" s="29" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="12"/>
@@ -26898,65 +26901,65 @@
       <c r="M20" s="12"/>
       <c r="N20" s="13"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
-      <c r="B21" s="28" t="s">
+    <row r="21" spans="1:14">
+      <c r="A21" s="40"/>
+      <c r="B21" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
       <c r="N21" s="11"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="28" t="s">
+    <row r="22" spans="1:14">
+      <c r="A22" s="40"/>
+      <c r="B22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
       <c r="N22" s="11"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
-      <c r="B23" s="28" t="s">
+    <row r="23" spans="1:14">
+      <c r="A23" s="40"/>
+      <c r="B23" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="30">
         <v>0.72</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="43"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="38"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
-      <c r="B24" s="28" t="s">
+    <row r="24" spans="1:14">
+      <c r="A24" s="40"/>
+      <c r="B24" s="29" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="27"/>
@@ -26970,10 +26973,10 @@
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
-      <c r="N24" s="29"/>
+      <c r="N24" s="28"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="32"/>
+    <row r="25" spans="1:14">
+      <c r="A25" s="41"/>
       <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
@@ -27010,14 +27013,14 @@
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -27046,7 +27049,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -27056,7 +27059,7 @@
       <c r="C2" s="20">
         <v>0.94899999999999995</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1">
@@ -27068,7 +27071,7 @@
       <c r="H2" s="20">
         <v>0.89500000000000002</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="43" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="1">
@@ -27080,11 +27083,11 @@
       <c r="M2" s="20">
         <v>0.91100000000000003</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -27094,7 +27097,7 @@
       <c r="C3" s="20">
         <v>0.84</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="43"/>
       <c r="F3" s="1">
         <v>1</v>
       </c>
@@ -27104,7 +27107,7 @@
       <c r="H3" s="20">
         <v>0.93100000000000005</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="43"/>
       <c r="K3" s="1">
         <v>1</v>
       </c>
@@ -27114,9 +27117,9 @@
       <c r="M3" s="20">
         <v>0.90900000000000003</v>
       </c>
-      <c r="N3" s="34"/>
+      <c r="N3" s="43"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -27126,7 +27129,7 @@
       <c r="C4" s="20">
         <v>0.876</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="43"/>
       <c r="F4" s="1">
         <v>2</v>
       </c>
@@ -27136,7 +27139,7 @@
       <c r="H4" s="20">
         <v>0.873</v>
       </c>
-      <c r="I4" s="34"/>
+      <c r="I4" s="43"/>
       <c r="K4" s="1">
         <v>2</v>
       </c>
@@ -27146,9 +27149,9 @@
       <c r="M4" s="20">
         <v>0.90100000000000002</v>
       </c>
-      <c r="N4" s="34"/>
+      <c r="N4" s="43"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -27158,7 +27161,7 @@
       <c r="C5" s="20">
         <v>0.93600000000000005</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="43"/>
       <c r="F5" s="1">
         <v>3</v>
       </c>
@@ -27168,7 +27171,7 @@
       <c r="H5" s="20">
         <v>0.83799999999999997</v>
       </c>
-      <c r="I5" s="34"/>
+      <c r="I5" s="43"/>
       <c r="K5" s="1">
         <v>3</v>
       </c>
@@ -27178,9 +27181,9 @@
       <c r="M5" s="20">
         <v>0.88400000000000001</v>
       </c>
-      <c r="N5" s="34"/>
+      <c r="N5" s="43"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -27190,7 +27193,7 @@
       <c r="C6" s="20">
         <v>0.97</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="43"/>
       <c r="F6" s="1">
         <v>4</v>
       </c>
@@ -27200,7 +27203,7 @@
       <c r="H6" s="20">
         <v>0.97799999999999998</v>
       </c>
-      <c r="I6" s="34"/>
+      <c r="I6" s="43"/>
       <c r="K6" s="1">
         <v>4</v>
       </c>
@@ -27210,9 +27213,9 @@
       <c r="M6" s="20">
         <v>0.93899999999999995</v>
       </c>
-      <c r="N6" s="34"/>
+      <c r="N6" s="43"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -27222,7 +27225,7 @@
       <c r="C7" s="20">
         <v>0.97199999999999998</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="43"/>
       <c r="F7" s="1">
         <v>5</v>
       </c>
@@ -27232,7 +27235,7 @@
       <c r="H7" s="20">
         <v>0.97899999999999998</v>
       </c>
-      <c r="I7" s="34"/>
+      <c r="I7" s="43"/>
       <c r="K7" s="1">
         <v>5</v>
       </c>
@@ -27242,9 +27245,9 @@
       <c r="M7" s="20">
         <v>0.91700000000000004</v>
       </c>
-      <c r="N7" s="34"/>
+      <c r="N7" s="43"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -27254,7 +27257,7 @@
       <c r="C8" s="20">
         <v>0.97399999999999998</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="43"/>
       <c r="F8" s="1">
         <v>6</v>
       </c>
@@ -27264,7 +27267,7 @@
       <c r="H8" s="20">
         <v>0.97199999999999998</v>
       </c>
-      <c r="I8" s="34"/>
+      <c r="I8" s="43"/>
       <c r="K8" s="1">
         <v>6</v>
       </c>
@@ -27274,9 +27277,9 @@
       <c r="M8" s="20">
         <v>0.92300000000000004</v>
       </c>
-      <c r="N8" s="34"/>
+      <c r="N8" s="43"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -27286,7 +27289,7 @@
       <c r="C9" s="20">
         <v>0.97799999999999998</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="43"/>
       <c r="F9" s="1">
         <v>7</v>
       </c>
@@ -27296,13 +27299,13 @@
       <c r="H9" s="20">
         <v>0.96499999999999997</v>
       </c>
-      <c r="I9" s="34"/>
+      <c r="I9" s="43"/>
       <c r="K9" s="1"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -27312,7 +27315,7 @@
       <c r="C10" s="20">
         <v>0.97799999999999998</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="43"/>
       <c r="F10" s="1">
         <v>8</v>
       </c>
@@ -27322,13 +27325,13 @@
       <c r="H10" s="20">
         <v>0.94899999999999995</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="43"/>
       <c r="K10" s="1"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="19"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -27338,7 +27341,7 @@
       <c r="C11" s="20">
         <v>0.97799999999999998</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="43"/>
       <c r="F11" s="1">
         <v>9</v>
       </c>
@@ -27348,13 +27351,13 @@
       <c r="H11" s="20">
         <v>0.93</v>
       </c>
-      <c r="I11" s="34"/>
+      <c r="I11" s="43"/>
       <c r="K11" s="1"/>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="19"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -27364,7 +27367,7 @@
       <c r="C12" s="20">
         <v>0.98099999999999998</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="43"/>
       <c r="F12" s="1">
         <v>10</v>
       </c>
@@ -27374,13 +27377,13 @@
       <c r="H12" s="20">
         <v>0.91500000000000004</v>
       </c>
-      <c r="I12" s="34"/>
+      <c r="I12" s="43"/>
       <c r="K12" s="1"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="19"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -27390,7 +27393,7 @@
       <c r="C13" s="20">
         <v>0.97899999999999998</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="43"/>
       <c r="F13" s="1">
         <v>11</v>
       </c>
@@ -27400,13 +27403,13 @@
       <c r="H13" s="20">
         <v>0.91500000000000004</v>
       </c>
-      <c r="I13" s="34"/>
+      <c r="I13" s="43"/>
       <c r="K13" s="1"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="19"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -27416,7 +27419,7 @@
       <c r="C14" s="20">
         <v>0.97399999999999998</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="43"/>
       <c r="F14" s="1">
         <v>12</v>
       </c>
@@ -27426,13 +27429,13 @@
       <c r="H14" s="20">
         <v>0.91900000000000004</v>
       </c>
-      <c r="I14" s="34"/>
+      <c r="I14" s="43"/>
       <c r="K14" s="1"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="19"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -27461,7 +27464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -27471,7 +27474,7 @@
       <c r="C34" s="20">
         <v>0.98199999999999998</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="43" t="s">
         <v>20</v>
       </c>
       <c r="F34" s="1">
@@ -27483,7 +27486,7 @@
       <c r="H34" s="20">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I34" s="34" t="s">
+      <c r="I34" s="43" t="s">
         <v>21</v>
       </c>
       <c r="K34" s="1">
@@ -27495,11 +27498,11 @@
       <c r="M34" s="20">
         <v>0.99399999999999999</v>
       </c>
-      <c r="N34" s="34" t="s">
+      <c r="N34" s="43" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -27509,7 +27512,7 @@
       <c r="C35" s="20">
         <v>0.91800000000000004</v>
       </c>
-      <c r="D35" s="34"/>
+      <c r="D35" s="43"/>
       <c r="F35" s="1">
         <v>1</v>
       </c>
@@ -27519,7 +27522,7 @@
       <c r="H35" s="20">
         <v>0.96399999999999997</v>
       </c>
-      <c r="I35" s="34"/>
+      <c r="I35" s="43"/>
       <c r="K35" s="1">
         <v>1</v>
       </c>
@@ -27529,9 +27532,9 @@
       <c r="M35" s="20">
         <v>0.99099999999999999</v>
       </c>
-      <c r="N35" s="34"/>
+      <c r="N35" s="43"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -27541,7 +27544,7 @@
       <c r="C36" s="20">
         <v>0.91900000000000004</v>
       </c>
-      <c r="D36" s="34"/>
+      <c r="D36" s="43"/>
       <c r="F36" s="1">
         <v>2</v>
       </c>
@@ -27551,7 +27554,7 @@
       <c r="H36" s="20">
         <v>0.97</v>
       </c>
-      <c r="I36" s="34"/>
+      <c r="I36" s="43"/>
       <c r="K36" s="1">
         <v>2</v>
       </c>
@@ -27561,9 +27564,9 @@
       <c r="M36" s="20">
         <v>0.98299999999999998</v>
       </c>
-      <c r="N36" s="34"/>
+      <c r="N36" s="43"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14">
       <c r="A37" s="1">
         <v>3</v>
       </c>
@@ -27573,7 +27576,7 @@
       <c r="C37" s="20">
         <v>0.97899999999999998</v>
       </c>
-      <c r="D37" s="34"/>
+      <c r="D37" s="43"/>
       <c r="F37" s="1">
         <v>3</v>
       </c>
@@ -27583,7 +27586,7 @@
       <c r="H37" s="20">
         <v>0.96599999999999997</v>
       </c>
-      <c r="I37" s="34"/>
+      <c r="I37" s="43"/>
       <c r="K37" s="1">
         <v>3</v>
       </c>
@@ -27593,9 +27596,9 @@
       <c r="M37" s="20">
         <v>0.98</v>
       </c>
-      <c r="N37" s="34"/>
+      <c r="N37" s="43"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -27605,7 +27608,7 @@
       <c r="C38" s="20">
         <v>0.97699999999999998</v>
       </c>
-      <c r="D38" s="34"/>
+      <c r="D38" s="43"/>
       <c r="F38" s="1">
         <v>4</v>
       </c>
@@ -27615,7 +27618,7 @@
       <c r="H38" s="20">
         <v>0.96799999999999997</v>
       </c>
-      <c r="I38" s="34"/>
+      <c r="I38" s="43"/>
       <c r="K38" s="1">
         <v>4</v>
       </c>
@@ -27625,9 +27628,9 @@
       <c r="M38" s="20">
         <v>0.97099999999999997</v>
       </c>
-      <c r="N38" s="34"/>
+      <c r="N38" s="43"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14">
       <c r="A39" s="1">
         <v>5</v>
       </c>
@@ -27637,7 +27640,7 @@
       <c r="C39" s="20">
         <v>0.98199999999999998</v>
       </c>
-      <c r="D39" s="34"/>
+      <c r="D39" s="43"/>
       <c r="F39" s="1">
         <v>5</v>
       </c>
@@ -27647,7 +27650,7 @@
       <c r="H39" s="20">
         <v>0.96699999999999997</v>
       </c>
-      <c r="I39" s="34"/>
+      <c r="I39" s="43"/>
       <c r="K39" s="1">
         <v>5</v>
       </c>
@@ -27657,9 +27660,9 @@
       <c r="M39" s="20">
         <v>0.873</v>
       </c>
-      <c r="N39" s="34"/>
+      <c r="N39" s="43"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14">
       <c r="A40" s="1">
         <v>6</v>
       </c>
@@ -27669,7 +27672,7 @@
       <c r="C40" s="20">
         <v>0.94399999999999995</v>
       </c>
-      <c r="D40" s="34"/>
+      <c r="D40" s="43"/>
       <c r="F40" s="1">
         <v>6</v>
       </c>
@@ -27679,7 +27682,7 @@
       <c r="H40" s="20">
         <v>0.96399999999999997</v>
       </c>
-      <c r="I40" s="34"/>
+      <c r="I40" s="43"/>
       <c r="K40" s="1">
         <v>6</v>
       </c>
@@ -27689,9 +27692,9 @@
       <c r="M40" s="20">
         <v>0.97899999999999998</v>
       </c>
-      <c r="N40" s="34"/>
+      <c r="N40" s="43"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14">
       <c r="A41" s="1">
         <v>7</v>
       </c>
@@ -27701,7 +27704,7 @@
       <c r="C41" s="20">
         <v>0.99299999999999999</v>
       </c>
-      <c r="D41" s="34"/>
+      <c r="D41" s="43"/>
       <c r="F41" s="1">
         <v>7</v>
       </c>
@@ -27711,7 +27714,7 @@
       <c r="H41" s="20">
         <v>0.97399999999999998</v>
       </c>
-      <c r="I41" s="34"/>
+      <c r="I41" s="43"/>
       <c r="K41" s="1">
         <v>7</v>
       </c>
@@ -27721,9 +27724,9 @@
       <c r="M41" s="20">
         <v>0.93</v>
       </c>
-      <c r="N41" s="34"/>
+      <c r="N41" s="43"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14">
       <c r="A42" s="1">
         <v>8</v>
       </c>
@@ -27733,7 +27736,7 @@
       <c r="C42" s="20">
         <v>0.94599999999999995</v>
       </c>
-      <c r="D42" s="34"/>
+      <c r="D42" s="43"/>
       <c r="F42" s="1">
         <v>8</v>
       </c>
@@ -27743,7 +27746,7 @@
       <c r="H42" s="20">
         <v>0.82099999999999995</v>
       </c>
-      <c r="I42" s="34"/>
+      <c r="I42" s="43"/>
       <c r="K42" s="1">
         <v>8</v>
       </c>
@@ -27753,9 +27756,9 @@
       <c r="M42" s="20">
         <v>0.98699999999999999</v>
       </c>
-      <c r="N42" s="34"/>
+      <c r="N42" s="43"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14">
       <c r="A43" s="1">
         <v>9</v>
       </c>
@@ -27765,7 +27768,7 @@
       <c r="C43" s="20">
         <v>0.98099999999999998</v>
       </c>
-      <c r="D43" s="34"/>
+      <c r="D43" s="43"/>
       <c r="F43" s="1">
         <v>9</v>
       </c>
@@ -27775,7 +27778,7 @@
       <c r="H43" s="20">
         <v>0.82799999999999996</v>
       </c>
-      <c r="I43" s="34"/>
+      <c r="I43" s="43"/>
       <c r="K43" s="1">
         <v>9</v>
       </c>
@@ -27785,9 +27788,9 @@
       <c r="M43" s="20">
         <v>0.93500000000000005</v>
       </c>
-      <c r="N43" s="34"/>
+      <c r="N43" s="43"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14">
       <c r="A44" s="1">
         <v>10</v>
       </c>
@@ -27797,7 +27800,7 @@
       <c r="C44" s="20">
         <v>0.98399999999999999</v>
       </c>
-      <c r="D44" s="34"/>
+      <c r="D44" s="43"/>
       <c r="F44" s="1">
         <v>10</v>
       </c>
@@ -27807,7 +27810,7 @@
       <c r="H44" s="20">
         <v>0.84099999999999997</v>
       </c>
-      <c r="I44" s="34"/>
+      <c r="I44" s="43"/>
       <c r="K44" s="1">
         <v>10</v>
       </c>
@@ -27817,9 +27820,9 @@
       <c r="M44" s="20">
         <v>0.92500000000000004</v>
       </c>
-      <c r="N44" s="34"/>
+      <c r="N44" s="43"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14">
       <c r="A45" s="1">
         <v>11</v>
       </c>
@@ -27829,7 +27832,7 @@
       <c r="C45" s="20">
         <v>0.95299999999999996</v>
       </c>
-      <c r="D45" s="34"/>
+      <c r="D45" s="43"/>
       <c r="F45" s="1">
         <v>11</v>
       </c>
@@ -27839,7 +27842,7 @@
       <c r="H45" s="20">
         <v>0.98</v>
       </c>
-      <c r="I45" s="34"/>
+      <c r="I45" s="43"/>
       <c r="K45" s="1">
         <v>11</v>
       </c>
@@ -27849,9 +27852,9 @@
       <c r="M45" s="20">
         <v>0.92400000000000004</v>
       </c>
-      <c r="N45" s="34"/>
+      <c r="N45" s="43"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14">
       <c r="A46" s="1">
         <v>12</v>
       </c>
@@ -27861,7 +27864,7 @@
       <c r="C46" s="20">
         <v>0.92100000000000004</v>
       </c>
-      <c r="D46" s="34"/>
+      <c r="D46" s="43"/>
       <c r="F46" s="1">
         <v>12</v>
       </c>
@@ -27871,7 +27874,7 @@
       <c r="H46" s="20">
         <v>0.84</v>
       </c>
-      <c r="I46" s="34"/>
+      <c r="I46" s="43"/>
       <c r="K46" s="1">
         <v>12</v>
       </c>
@@ -27881,9 +27884,9 @@
       <c r="M46" s="20">
         <v>0.93300000000000005</v>
       </c>
-      <c r="N46" s="34"/>
+      <c r="N46" s="43"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14">
       <c r="A66" s="1" t="s">
         <v>33</v>
       </c>
@@ -27912,7 +27915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14">
       <c r="A67" s="1">
         <v>0</v>
       </c>
@@ -27922,7 +27925,7 @@
       <c r="C67" s="20">
         <v>0.77700000000000002</v>
       </c>
-      <c r="D67" s="34" t="s">
+      <c r="D67" s="43" t="s">
         <v>23</v>
       </c>
       <c r="F67" s="1">
@@ -27934,7 +27937,7 @@
       <c r="H67" s="20">
         <v>0.75900000000000001</v>
       </c>
-      <c r="I67" s="34" t="s">
+      <c r="I67" s="43" t="s">
         <v>24</v>
       </c>
       <c r="K67" s="1">
@@ -27946,11 +27949,11 @@
       <c r="M67" s="20">
         <v>0.89400000000000002</v>
       </c>
-      <c r="N67" s="34" t="s">
+      <c r="N67" s="43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14">
       <c r="A68" s="1">
         <v>1</v>
       </c>
@@ -27960,7 +27963,7 @@
       <c r="C68" s="20">
         <v>0.85099999999999998</v>
       </c>
-      <c r="D68" s="34"/>
+      <c r="D68" s="43"/>
       <c r="F68" s="1">
         <v>1</v>
       </c>
@@ -27970,7 +27973,7 @@
       <c r="H68" s="20">
         <v>0.97399999999999998</v>
       </c>
-      <c r="I68" s="34"/>
+      <c r="I68" s="43"/>
       <c r="K68" s="1">
         <v>1</v>
       </c>
@@ -27980,9 +27983,9 @@
       <c r="M68" s="20">
         <v>0.94299999999999995</v>
       </c>
-      <c r="N68" s="34"/>
+      <c r="N68" s="43"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14">
       <c r="A69" s="1">
         <v>2</v>
       </c>
@@ -27992,7 +27995,7 @@
       <c r="C69" s="20">
         <v>0.93300000000000005</v>
       </c>
-      <c r="D69" s="34"/>
+      <c r="D69" s="43"/>
       <c r="F69" s="1">
         <v>2</v>
       </c>
@@ -28002,7 +28005,7 @@
       <c r="H69" s="20">
         <v>0.81899999999999995</v>
       </c>
-      <c r="I69" s="34"/>
+      <c r="I69" s="43"/>
       <c r="K69" s="1">
         <v>2</v>
       </c>
@@ -28012,9 +28015,9 @@
       <c r="M69" s="20">
         <v>0.97799999999999998</v>
       </c>
-      <c r="N69" s="34"/>
+      <c r="N69" s="43"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14">
       <c r="A70" s="1">
         <v>3</v>
       </c>
@@ -28024,7 +28027,7 @@
       <c r="C70" s="20">
         <v>0.92700000000000005</v>
       </c>
-      <c r="D70" s="34"/>
+      <c r="D70" s="43"/>
       <c r="F70" s="1">
         <v>3</v>
       </c>
@@ -28034,7 +28037,7 @@
       <c r="H70" s="20">
         <v>0.97199999999999998</v>
       </c>
-      <c r="I70" s="34"/>
+      <c r="I70" s="43"/>
       <c r="K70" s="1">
         <v>3</v>
       </c>
@@ -28044,9 +28047,9 @@
       <c r="M70" s="20">
         <v>0.97499999999999998</v>
       </c>
-      <c r="N70" s="34"/>
+      <c r="N70" s="43"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14">
       <c r="A71" s="1">
         <v>4</v>
       </c>
@@ -28056,7 +28059,7 @@
       <c r="C71" s="20">
         <v>0.90600000000000003</v>
       </c>
-      <c r="D71" s="34"/>
+      <c r="D71" s="43"/>
       <c r="F71" s="1">
         <v>4</v>
       </c>
@@ -28066,7 +28069,7 @@
       <c r="H71" s="20">
         <v>0.96899999999999997</v>
       </c>
-      <c r="I71" s="34"/>
+      <c r="I71" s="43"/>
       <c r="K71" s="1">
         <v>4</v>
       </c>
@@ -28076,9 +28079,9 @@
       <c r="M71" s="20">
         <v>0.85199999999999998</v>
       </c>
-      <c r="N71" s="34"/>
+      <c r="N71" s="43"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14">
       <c r="A72" s="1">
         <v>5</v>
       </c>
@@ -28088,7 +28091,7 @@
       <c r="C72" s="20">
         <v>0.92</v>
       </c>
-      <c r="D72" s="34"/>
+      <c r="D72" s="43"/>
       <c r="F72" s="1">
         <v>5</v>
       </c>
@@ -28098,7 +28101,7 @@
       <c r="H72" s="20">
         <v>0.96499999999999997</v>
       </c>
-      <c r="I72" s="34"/>
+      <c r="I72" s="43"/>
       <c r="K72" s="1">
         <v>5</v>
       </c>
@@ -28108,9 +28111,9 @@
       <c r="M72" s="20">
         <v>0.86899999999999999</v>
       </c>
-      <c r="N72" s="34"/>
+      <c r="N72" s="43"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14">
       <c r="A73" s="1">
         <v>6</v>
       </c>
@@ -28120,7 +28123,7 @@
       <c r="C73" s="20">
         <v>0.96199999999999997</v>
       </c>
-      <c r="D73" s="34"/>
+      <c r="D73" s="43"/>
       <c r="F73" s="1">
         <v>6</v>
       </c>
@@ -28130,7 +28133,7 @@
       <c r="H73" s="20">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I73" s="34"/>
+      <c r="I73" s="43"/>
       <c r="K73" s="1">
         <v>6</v>
       </c>
@@ -28140,9 +28143,9 @@
       <c r="M73" s="20">
         <v>0.876</v>
       </c>
-      <c r="N73" s="34"/>
+      <c r="N73" s="43"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14">
       <c r="A74" s="1">
         <v>7</v>
       </c>
@@ -28152,7 +28155,7 @@
       <c r="C74" s="20">
         <v>0.82199999999999995</v>
       </c>
-      <c r="D74" s="34"/>
+      <c r="D74" s="43"/>
       <c r="F74" s="1">
         <v>7</v>
       </c>
@@ -28162,7 +28165,7 @@
       <c r="H74" s="20">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I74" s="34"/>
+      <c r="I74" s="43"/>
       <c r="K74" s="1">
         <v>7</v>
       </c>
@@ -28172,9 +28175,9 @@
       <c r="M74" s="20">
         <v>0.89300000000000002</v>
       </c>
-      <c r="N74" s="34"/>
+      <c r="N74" s="43"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14">
       <c r="A75" s="1">
         <v>8</v>
       </c>
@@ -28184,7 +28187,7 @@
       <c r="C75" s="20">
         <v>0.82399999999999995</v>
       </c>
-      <c r="D75" s="34"/>
+      <c r="D75" s="43"/>
       <c r="F75" s="1">
         <v>8</v>
       </c>
@@ -28194,7 +28197,7 @@
       <c r="H75" s="20">
         <v>0.91800000000000004</v>
       </c>
-      <c r="I75" s="34"/>
+      <c r="I75" s="43"/>
       <c r="K75" s="1">
         <v>8</v>
       </c>
@@ -28204,9 +28207,9 @@
       <c r="M75" s="20">
         <v>0.98799999999999999</v>
       </c>
-      <c r="N75" s="34"/>
+      <c r="N75" s="43"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14">
       <c r="A76" s="1">
         <v>9</v>
       </c>
@@ -28216,7 +28219,7 @@
       <c r="C76" s="20">
         <v>0.92500000000000004</v>
       </c>
-      <c r="D76" s="34"/>
+      <c r="D76" s="43"/>
       <c r="F76" s="1">
         <v>9</v>
       </c>
@@ -28226,7 +28229,7 @@
       <c r="H76" s="20">
         <v>0.97899999999999998</v>
       </c>
-      <c r="I76" s="34"/>
+      <c r="I76" s="43"/>
       <c r="K76" s="1">
         <v>9</v>
       </c>
@@ -28236,9 +28239,9 @@
       <c r="M76" s="20">
         <v>0.89500000000000002</v>
       </c>
-      <c r="N76" s="34"/>
+      <c r="N76" s="43"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14">
       <c r="A77" s="1">
         <v>10</v>
       </c>
@@ -28248,7 +28251,7 @@
       <c r="C77" s="20">
         <v>0.83199999999999996</v>
       </c>
-      <c r="D77" s="34"/>
+      <c r="D77" s="43"/>
       <c r="F77" s="1">
         <v>10</v>
       </c>
@@ -28258,7 +28261,7 @@
       <c r="H77" s="20">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I77" s="34"/>
+      <c r="I77" s="43"/>
       <c r="K77" s="1">
         <v>10</v>
       </c>
@@ -28268,9 +28271,9 @@
       <c r="M77" s="20">
         <v>0.98199999999999998</v>
       </c>
-      <c r="N77" s="34"/>
+      <c r="N77" s="43"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14">
       <c r="A78" s="1">
         <v>11</v>
       </c>
@@ -28280,7 +28283,7 @@
       <c r="C78" s="20">
         <v>0.82899999999999996</v>
       </c>
-      <c r="D78" s="34"/>
+      <c r="D78" s="43"/>
       <c r="F78" s="1">
         <v>11</v>
       </c>
@@ -28290,7 +28293,7 @@
       <c r="H78" s="20">
         <v>0.94899999999999995</v>
       </c>
-      <c r="I78" s="34"/>
+      <c r="I78" s="43"/>
       <c r="K78" s="1">
         <v>11</v>
       </c>
@@ -28300,9 +28303,9 @@
       <c r="M78" s="20">
         <v>0.98099999999999998</v>
       </c>
-      <c r="N78" s="34"/>
+      <c r="N78" s="43"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14">
       <c r="A79" s="1">
         <v>12</v>
       </c>
@@ -28312,7 +28315,7 @@
       <c r="C79" s="20">
         <v>0.95399999999999996</v>
       </c>
-      <c r="D79" s="34"/>
+      <c r="D79" s="43"/>
       <c r="F79" s="1">
         <v>12</v>
       </c>
@@ -28322,7 +28325,7 @@
       <c r="H79" s="20">
         <v>0.99299999999999999</v>
       </c>
-      <c r="I79" s="34"/>
+      <c r="I79" s="43"/>
       <c r="K79" s="1">
         <v>12</v>
       </c>
@@ -28332,9 +28335,9 @@
       <c r="M79" s="20">
         <v>0.95899999999999996</v>
       </c>
-      <c r="N79" s="34"/>
+      <c r="N79" s="43"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14">
       <c r="A98" s="1" t="s">
         <v>33</v>
       </c>
@@ -28363,7 +28366,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14">
       <c r="A99" s="1">
         <v>0</v>
       </c>
@@ -28373,7 +28376,7 @@
       <c r="C99" s="20">
         <v>0.92200000000000004</v>
       </c>
-      <c r="D99" s="34" t="s">
+      <c r="D99" s="43" t="s">
         <v>26</v>
       </c>
       <c r="F99" s="1">
@@ -28385,7 +28388,7 @@
       <c r="H99" s="20">
         <v>0.874</v>
       </c>
-      <c r="I99" s="34" t="s">
+      <c r="I99" s="43" t="s">
         <v>27</v>
       </c>
       <c r="K99" s="1">
@@ -28397,11 +28400,11 @@
       <c r="M99" s="20">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N99" s="34" t="s">
+      <c r="N99" s="43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14">
       <c r="A100" s="1">
         <v>1</v>
       </c>
@@ -28411,7 +28414,7 @@
       <c r="C100" s="20">
         <v>0.91600000000000004</v>
       </c>
-      <c r="D100" s="34"/>
+      <c r="D100" s="43"/>
       <c r="F100" s="1">
         <v>1</v>
       </c>
@@ -28421,7 +28424,7 @@
       <c r="H100" s="20">
         <v>0.89500000000000002</v>
       </c>
-      <c r="I100" s="34"/>
+      <c r="I100" s="43"/>
       <c r="K100" s="1">
         <v>1</v>
       </c>
@@ -28431,9 +28434,9 @@
       <c r="M100" s="20">
         <v>0.98499999999999999</v>
       </c>
-      <c r="N100" s="34"/>
+      <c r="N100" s="43"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14">
       <c r="A101" s="1">
         <v>2</v>
       </c>
@@ -28443,7 +28446,7 @@
       <c r="C101" s="20">
         <v>0.89200000000000002</v>
       </c>
-      <c r="D101" s="34"/>
+      <c r="D101" s="43"/>
       <c r="F101" s="1">
         <v>2</v>
       </c>
@@ -28453,7 +28456,7 @@
       <c r="H101" s="20">
         <v>0.96299999999999997</v>
       </c>
-      <c r="I101" s="34"/>
+      <c r="I101" s="43"/>
       <c r="K101" s="1">
         <v>2</v>
       </c>
@@ -28463,9 +28466,9 @@
       <c r="M101" s="20">
         <v>0.96699999999999997</v>
       </c>
-      <c r="N101" s="34"/>
+      <c r="N101" s="43"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14">
       <c r="A102" s="1">
         <v>3</v>
       </c>
@@ -28475,7 +28478,7 @@
       <c r="C102" s="20">
         <v>0.91</v>
       </c>
-      <c r="D102" s="34"/>
+      <c r="D102" s="43"/>
       <c r="F102" s="1">
         <v>3</v>
       </c>
@@ -28485,7 +28488,7 @@
       <c r="H102" s="20">
         <v>0.97199999999999998</v>
       </c>
-      <c r="I102" s="34"/>
+      <c r="I102" s="43"/>
       <c r="K102" s="1">
         <v>3</v>
       </c>
@@ -28495,9 +28498,9 @@
       <c r="M102" s="20">
         <v>0.995</v>
       </c>
-      <c r="N102" s="34"/>
+      <c r="N102" s="43"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14">
       <c r="A103" s="1">
         <v>4</v>
       </c>
@@ -28507,7 +28510,7 @@
       <c r="C103" s="20">
         <v>0.89800000000000002</v>
       </c>
-      <c r="D103" s="34"/>
+      <c r="D103" s="43"/>
       <c r="F103" s="1">
         <v>4</v>
       </c>
@@ -28517,7 +28520,7 @@
       <c r="H103" s="20">
         <v>0.98399999999999999</v>
       </c>
-      <c r="I103" s="34"/>
+      <c r="I103" s="43"/>
       <c r="K103" s="1">
         <v>4</v>
       </c>
@@ -28527,9 +28530,9 @@
       <c r="M103" s="20">
         <v>0.98699999999999999</v>
       </c>
-      <c r="N103" s="34"/>
+      <c r="N103" s="43"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14">
       <c r="A104" s="1">
         <v>5</v>
       </c>
@@ -28539,7 +28542,7 @@
       <c r="C104" s="20">
         <v>0.88</v>
       </c>
-      <c r="D104" s="34"/>
+      <c r="D104" s="43"/>
       <c r="F104" s="1">
         <v>5</v>
       </c>
@@ -28549,7 +28552,7 @@
       <c r="H104" s="20">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I104" s="34"/>
+      <c r="I104" s="43"/>
       <c r="K104" s="1">
         <v>5</v>
       </c>
@@ -28559,9 +28562,9 @@
       <c r="M104" s="20">
         <v>0.996</v>
       </c>
-      <c r="N104" s="34"/>
+      <c r="N104" s="43"/>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14">
       <c r="A105" s="1">
         <v>6</v>
       </c>
@@ -28571,7 +28574,7 @@
       <c r="C105" s="20">
         <v>0.90400000000000003</v>
       </c>
-      <c r="D105" s="34"/>
+      <c r="D105" s="43"/>
       <c r="F105" s="1">
         <v>6</v>
       </c>
@@ -28581,7 +28584,7 @@
       <c r="H105" s="20">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I105" s="34"/>
+      <c r="I105" s="43"/>
       <c r="K105" s="1">
         <v>6</v>
       </c>
@@ -28591,9 +28594,9 @@
       <c r="M105" s="20">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N105" s="34"/>
+      <c r="N105" s="43"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14">
       <c r="A106" s="1">
         <v>7</v>
       </c>
@@ -28603,7 +28606,7 @@
       <c r="C106" s="20">
         <v>0.96699999999999997</v>
       </c>
-      <c r="D106" s="34"/>
+      <c r="D106" s="43"/>
       <c r="F106" s="1">
         <v>7</v>
       </c>
@@ -28613,7 +28616,7 @@
       <c r="H106" s="20">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I106" s="34"/>
+      <c r="I106" s="43"/>
       <c r="K106" s="1">
         <v>7</v>
       </c>
@@ -28623,9 +28626,9 @@
       <c r="M106" s="20">
         <v>0.98899999999999999</v>
       </c>
-      <c r="N106" s="34"/>
+      <c r="N106" s="43"/>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14">
       <c r="A107" s="1">
         <v>8</v>
       </c>
@@ -28635,7 +28638,7 @@
       <c r="C107" s="20">
         <v>0.97399999999999998</v>
       </c>
-      <c r="D107" s="34"/>
+      <c r="D107" s="43"/>
       <c r="F107" s="1">
         <v>8</v>
       </c>
@@ -28645,7 +28648,7 @@
       <c r="H107" s="20">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I107" s="34"/>
+      <c r="I107" s="43"/>
       <c r="K107" s="1">
         <v>8</v>
       </c>
@@ -28655,9 +28658,9 @@
       <c r="M107" s="20">
         <v>0.96099999999999997</v>
       </c>
-      <c r="N107" s="34"/>
+      <c r="N107" s="43"/>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14">
       <c r="A108" s="1">
         <v>9</v>
       </c>
@@ -28667,7 +28670,7 @@
       <c r="C108" s="20">
         <v>0.97799999999999998</v>
       </c>
-      <c r="D108" s="34"/>
+      <c r="D108" s="43"/>
       <c r="F108" s="1">
         <v>9</v>
       </c>
@@ -28677,7 +28680,7 @@
       <c r="H108" s="20">
         <v>0.89900000000000002</v>
       </c>
-      <c r="I108" s="34"/>
+      <c r="I108" s="43"/>
       <c r="K108" s="1">
         <v>9</v>
       </c>
@@ -28687,9 +28690,9 @@
       <c r="M108" s="20">
         <v>0.96</v>
       </c>
-      <c r="N108" s="34"/>
+      <c r="N108" s="43"/>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14">
       <c r="A109" s="1">
         <v>10</v>
       </c>
@@ -28699,7 +28702,7 @@
       <c r="C109" s="20">
         <v>0.97699999999999998</v>
       </c>
-      <c r="D109" s="34"/>
+      <c r="D109" s="43"/>
       <c r="F109" s="1">
         <v>10</v>
       </c>
@@ -28709,7 +28712,7 @@
       <c r="H109" s="20">
         <v>0.97199999999999998</v>
       </c>
-      <c r="I109" s="34"/>
+      <c r="I109" s="43"/>
       <c r="K109" s="1">
         <v>10</v>
       </c>
@@ -28719,9 +28722,9 @@
       <c r="M109" s="20">
         <v>0.96399999999999997</v>
       </c>
-      <c r="N109" s="34"/>
+      <c r="N109" s="43"/>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14">
       <c r="A110" s="1">
         <v>11</v>
       </c>
@@ -28731,7 +28734,7 @@
       <c r="C110" s="20">
         <v>0.97599999999999998</v>
       </c>
-      <c r="D110" s="34"/>
+      <c r="D110" s="43"/>
       <c r="F110" s="1">
         <v>11</v>
       </c>
@@ -28741,7 +28744,7 @@
       <c r="H110" s="20">
         <v>0.85599999999999998</v>
       </c>
-      <c r="I110" s="34"/>
+      <c r="I110" s="43"/>
       <c r="K110" s="1">
         <v>11</v>
       </c>
@@ -28751,9 +28754,9 @@
       <c r="M110" s="20">
         <v>0.96</v>
       </c>
-      <c r="N110" s="34"/>
+      <c r="N110" s="43"/>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14">
       <c r="A111" s="1">
         <v>12</v>
       </c>
@@ -28763,7 +28766,7 @@
       <c r="C111" s="20">
         <v>0.97899999999999998</v>
       </c>
-      <c r="D111" s="34"/>
+      <c r="D111" s="43"/>
       <c r="F111" s="1">
         <v>12</v>
       </c>
@@ -28773,7 +28776,7 @@
       <c r="H111" s="20">
         <v>0.97399999999999998</v>
       </c>
-      <c r="I111" s="34"/>
+      <c r="I111" s="43"/>
       <c r="K111" s="1">
         <v>12</v>
       </c>
@@ -28783,22 +28786,22 @@
       <c r="M111" s="20">
         <v>0.96599999999999997</v>
       </c>
-      <c r="N111" s="34"/>
+      <c r="N111" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D2:D14"/>
+    <mergeCell ref="I2:I14"/>
+    <mergeCell ref="N2:N8"/>
+    <mergeCell ref="D34:D46"/>
+    <mergeCell ref="I34:I46"/>
+    <mergeCell ref="N34:N46"/>
     <mergeCell ref="D67:D79"/>
     <mergeCell ref="I67:I79"/>
     <mergeCell ref="N67:N79"/>
     <mergeCell ref="D99:D111"/>
     <mergeCell ref="I99:I111"/>
     <mergeCell ref="N99:N111"/>
-    <mergeCell ref="D2:D14"/>
-    <mergeCell ref="I2:I14"/>
-    <mergeCell ref="N2:N8"/>
-    <mergeCell ref="D34:D46"/>
-    <mergeCell ref="I34:I46"/>
-    <mergeCell ref="N34:N46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -28813,12 +28816,12 @@
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -28847,7 +28850,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -28857,7 +28860,7 @@
       <c r="C2" s="24">
         <v>0.66666700000000001</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="43" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="1">
@@ -28869,7 +28872,7 @@
       <c r="H2" s="24">
         <v>0</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="43" t="s">
         <v>28</v>
       </c>
       <c r="L2" s="1">
@@ -28881,11 +28884,11 @@
       <c r="N2" s="24">
         <v>0.66666700000000001</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -28895,7 +28898,7 @@
       <c r="C3" s="24">
         <v>0.51964299999999997</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="43"/>
       <c r="F3" s="1">
         <v>1</v>
       </c>
@@ -28905,7 +28908,7 @@
       <c r="H3" s="24">
         <v>9.1979999999999996E-3</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="43"/>
       <c r="L3" s="1">
         <v>1</v>
       </c>
@@ -28915,9 +28918,9 @@
       <c r="N3" s="24">
         <v>0.61618799999999996</v>
       </c>
-      <c r="O3" s="34"/>
+      <c r="O3" s="43"/>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -28927,7 +28930,7 @@
       <c r="C4" s="24">
         <v>0.54270200000000002</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="43"/>
       <c r="F4" s="1">
         <v>2</v>
       </c>
@@ -28937,7 +28940,7 @@
       <c r="H4" s="24">
         <v>0.66666700000000001</v>
       </c>
-      <c r="I4" s="34"/>
+      <c r="I4" s="43"/>
       <c r="L4" s="1">
         <v>2</v>
       </c>
@@ -28947,9 +28950,9 @@
       <c r="N4" s="24">
         <v>8.9940999999999993E-2</v>
       </c>
-      <c r="O4" s="34"/>
+      <c r="O4" s="43"/>
     </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -28959,7 +28962,7 @@
       <c r="C5" s="24">
         <v>0.58758500000000002</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="43"/>
       <c r="F5" s="1">
         <v>3</v>
       </c>
@@ -28969,7 +28972,7 @@
       <c r="H5" s="24">
         <v>0.66666700000000001</v>
       </c>
-      <c r="I5" s="34"/>
+      <c r="I5" s="43"/>
       <c r="L5" s="1">
         <v>3</v>
       </c>
@@ -28979,9 +28982,9 @@
       <c r="N5" s="24">
         <v>0</v>
       </c>
-      <c r="O5" s="34"/>
+      <c r="O5" s="43"/>
     </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -28991,7 +28994,7 @@
       <c r="C6" s="24">
         <v>0.59606400000000004</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="43"/>
       <c r="F6" s="1">
         <v>4</v>
       </c>
@@ -29001,7 +29004,7 @@
       <c r="H6" s="24">
         <v>0</v>
       </c>
-      <c r="I6" s="34"/>
+      <c r="I6" s="43"/>
       <c r="L6" s="1">
         <v>4</v>
       </c>
@@ -29011,9 +29014,9 @@
       <c r="N6" s="24">
         <v>0</v>
       </c>
-      <c r="O6" s="34"/>
+      <c r="O6" s="43"/>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -29023,7 +29026,7 @@
       <c r="C7" s="24">
         <v>0.63406600000000002</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="43"/>
       <c r="F7" s="1">
         <v>5</v>
       </c>
@@ -29033,7 +29036,7 @@
       <c r="H7" s="24">
         <v>0</v>
       </c>
-      <c r="I7" s="34"/>
+      <c r="I7" s="43"/>
       <c r="L7" s="1">
         <v>5</v>
       </c>
@@ -29043,9 +29046,9 @@
       <c r="N7" s="24">
         <v>0</v>
       </c>
-      <c r="O7" s="34"/>
+      <c r="O7" s="43"/>
     </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -29055,7 +29058,7 @@
       <c r="C8" s="24">
         <v>0.63100100000000003</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="43"/>
       <c r="F8" s="1">
         <v>6</v>
       </c>
@@ -29065,7 +29068,7 @@
       <c r="H8" s="24">
         <v>0</v>
       </c>
-      <c r="I8" s="34"/>
+      <c r="I8" s="43"/>
       <c r="L8" s="1">
         <v>6</v>
       </c>
@@ -29075,9 +29078,9 @@
       <c r="N8" s="24">
         <v>1.853E-3</v>
       </c>
-      <c r="O8" s="34"/>
+      <c r="O8" s="43"/>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -29087,7 +29090,7 @@
       <c r="C9" s="24">
         <v>0.62990500000000005</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="43"/>
       <c r="F9" s="1">
         <v>7</v>
       </c>
@@ -29097,7 +29100,7 @@
       <c r="H9" s="24">
         <v>0</v>
       </c>
-      <c r="I9" s="34"/>
+      <c r="I9" s="43"/>
       <c r="L9" s="1">
         <v>7</v>
       </c>
@@ -29107,9 +29110,9 @@
       <c r="N9" s="24">
         <v>4.8050000000000002E-3</v>
       </c>
-      <c r="O9" s="34"/>
+      <c r="O9" s="43"/>
     </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -29119,7 +29122,7 @@
       <c r="C10" s="24">
         <v>0.62997499999999995</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="43"/>
       <c r="F10" s="1">
         <v>8</v>
       </c>
@@ -29129,7 +29132,7 @@
       <c r="H10" s="24">
         <v>0</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="43"/>
       <c r="L10" s="1">
         <v>8</v>
       </c>
@@ -29139,9 +29142,9 @@
       <c r="N10" s="24">
         <v>9.9369999999999997E-3</v>
       </c>
-      <c r="O10" s="34"/>
+      <c r="O10" s="43"/>
     </row>
-    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -29151,7 +29154,7 @@
       <c r="C11" s="24">
         <v>0.629741</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="43"/>
       <c r="F11" s="1">
         <v>9</v>
       </c>
@@ -29161,7 +29164,7 @@
       <c r="H11" s="24">
         <v>0</v>
       </c>
-      <c r="I11" s="34"/>
+      <c r="I11" s="43"/>
       <c r="L11" s="1">
         <v>9</v>
       </c>
@@ -29171,9 +29174,9 @@
       <c r="N11" s="24">
         <v>7.0303000000000004E-2</v>
       </c>
-      <c r="O11" s="34"/>
+      <c r="O11" s="43"/>
     </row>
-    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -29183,7 +29186,7 @@
       <c r="C12" s="24">
         <v>0.62902800000000003</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="43"/>
       <c r="F12" s="1">
         <v>10</v>
       </c>
@@ -29193,7 +29196,7 @@
       <c r="H12" s="24">
         <v>0</v>
       </c>
-      <c r="I12" s="34"/>
+      <c r="I12" s="43"/>
       <c r="L12" s="1">
         <v>10</v>
       </c>
@@ -29203,9 +29206,9 @@
       <c r="N12" s="24">
         <v>0.25535999999999998</v>
       </c>
-      <c r="O12" s="34"/>
+      <c r="O12" s="43"/>
     </row>
-    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -29215,7 +29218,7 @@
       <c r="C13" s="24">
         <v>0.65797799999999995</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="43"/>
       <c r="F13" s="1">
         <v>11</v>
       </c>
@@ -29225,7 +29228,7 @@
       <c r="H13" s="24">
         <v>0</v>
       </c>
-      <c r="I13" s="34"/>
+      <c r="I13" s="43"/>
       <c r="L13" s="1">
         <v>11</v>
       </c>
@@ -29235,9 +29238,9 @@
       <c r="N13" s="24">
         <v>0.30926500000000001</v>
       </c>
-      <c r="O13" s="34"/>
+      <c r="O13" s="43"/>
     </row>
-    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -29247,7 +29250,7 @@
       <c r="C14" s="24">
         <v>0.57034200000000002</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="43"/>
       <c r="F14" s="1">
         <v>12</v>
       </c>
@@ -29257,7 +29260,7 @@
       <c r="H14" s="24">
         <v>0.212117</v>
       </c>
-      <c r="I14" s="34"/>
+      <c r="I14" s="43"/>
       <c r="L14" s="1">
         <v>12</v>
       </c>
@@ -29267,7 +29270,7 @@
       <c r="N14" s="24">
         <v>0.25233499999999998</v>
       </c>
-      <c r="O14" s="34"/>
+      <c r="O14" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -29288,13 +29291,13 @@
       <selection activeCell="K1" sqref="K1:M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -29323,7 +29326,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -29333,7 +29336,7 @@
       <c r="C2" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="43" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="1">
@@ -29345,7 +29348,7 @@
       <c r="H2" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="43" t="s">
         <v>28</v>
       </c>
       <c r="K2" s="1">
@@ -29357,11 +29360,11 @@
       <c r="M2" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -29371,7 +29374,7 @@
       <c r="C3" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="43"/>
       <c r="F3" s="1">
         <v>1</v>
       </c>
@@ -29381,7 +29384,7 @@
       <c r="H3" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="43"/>
       <c r="K3" s="1">
         <v>1</v>
       </c>
@@ -29391,9 +29394,9 @@
       <c r="M3" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="N3" s="34"/>
+      <c r="N3" s="43"/>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -29403,7 +29406,7 @@
       <c r="C4" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="43"/>
       <c r="F4" s="1">
         <v>2</v>
       </c>
@@ -29413,7 +29416,7 @@
       <c r="H4" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I4" s="34"/>
+      <c r="I4" s="43"/>
       <c r="K4" s="1">
         <v>2</v>
       </c>
@@ -29423,9 +29426,9 @@
       <c r="M4" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="N4" s="34"/>
+      <c r="N4" s="43"/>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -29435,7 +29438,7 @@
       <c r="C5" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="43"/>
       <c r="F5" s="1">
         <v>3</v>
       </c>
@@ -29445,7 +29448,7 @@
       <c r="H5" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I5" s="34"/>
+      <c r="I5" s="43"/>
       <c r="K5" s="1">
         <v>3</v>
       </c>
@@ -29455,9 +29458,9 @@
       <c r="M5" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="N5" s="34"/>
+      <c r="N5" s="43"/>
     </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -29467,7 +29470,7 @@
       <c r="C6" s="24">
         <v>0.480132</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="43"/>
       <c r="F6" s="1">
         <v>4</v>
       </c>
@@ -29477,7 +29480,7 @@
       <c r="H6" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I6" s="34"/>
+      <c r="I6" s="43"/>
       <c r="K6" s="1">
         <v>4</v>
       </c>
@@ -29487,9 +29490,9 @@
       <c r="M6" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="N6" s="34"/>
+      <c r="N6" s="43"/>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -29499,7 +29502,7 @@
       <c r="C7" s="24">
         <v>0.46854299999999999</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="43"/>
       <c r="F7" s="1">
         <v>5</v>
       </c>
@@ -29509,7 +29512,7 @@
       <c r="H7" s="24">
         <v>0.480132</v>
       </c>
-      <c r="I7" s="34"/>
+      <c r="I7" s="43"/>
       <c r="K7" s="1">
         <v>5</v>
       </c>
@@ -29519,9 +29522,9 @@
       <c r="M7" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="N7" s="34"/>
+      <c r="N7" s="43"/>
     </row>
-    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -29531,7 +29534,7 @@
       <c r="C8" s="24">
         <v>0.47682099999999999</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="43"/>
       <c r="F8" s="1">
         <v>6</v>
       </c>
@@ -29541,7 +29544,7 @@
       <c r="H8" s="24">
         <v>0.49337700000000001</v>
       </c>
-      <c r="I8" s="34"/>
+      <c r="I8" s="43"/>
       <c r="K8" s="1">
         <v>6</v>
       </c>
@@ -29551,9 +29554,9 @@
       <c r="M8" s="24">
         <v>0.48344399999999998</v>
       </c>
-      <c r="N8" s="34"/>
+      <c r="N8" s="43"/>
     </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -29563,7 +29566,7 @@
       <c r="C9" s="24">
         <v>0.480132</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="43"/>
       <c r="F9" s="1">
         <v>7</v>
       </c>
@@ -29573,7 +29576,7 @@
       <c r="H9" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I9" s="34"/>
+      <c r="I9" s="43"/>
       <c r="K9" s="1">
         <v>7</v>
       </c>
@@ -29583,9 +29586,9 @@
       <c r="M9" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="N9" s="34"/>
+      <c r="N9" s="43"/>
     </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -29595,7 +29598,7 @@
       <c r="C10" s="24">
         <v>0.480132</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="43"/>
       <c r="F10" s="1">
         <v>8</v>
       </c>
@@ -29605,7 +29608,7 @@
       <c r="H10" s="24">
         <v>0.480132</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="43"/>
       <c r="K10" s="1">
         <v>8</v>
       </c>
@@ -29615,9 +29618,9 @@
       <c r="M10" s="24">
         <v>0.47847699999999999</v>
       </c>
-      <c r="N10" s="34"/>
+      <c r="N10" s="43"/>
     </row>
-    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -29627,7 +29630,7 @@
       <c r="C11" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="43"/>
       <c r="F11" s="1">
         <v>9</v>
       </c>
@@ -29637,7 +29640,7 @@
       <c r="H11" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I11" s="34"/>
+      <c r="I11" s="43"/>
       <c r="K11" s="1">
         <v>9</v>
       </c>
@@ -29647,9 +29650,9 @@
       <c r="M11" s="24">
         <v>0.47682099999999999</v>
       </c>
-      <c r="N11" s="34"/>
+      <c r="N11" s="43"/>
     </row>
-    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -29659,7 +29662,7 @@
       <c r="C12" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="43"/>
       <c r="F12" s="1">
         <v>10</v>
       </c>
@@ -29669,7 +29672,7 @@
       <c r="H12" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I12" s="34"/>
+      <c r="I12" s="43"/>
       <c r="K12" s="1">
         <v>10</v>
       </c>
@@ -29679,9 +29682,9 @@
       <c r="M12" s="24">
         <v>0.47682099999999999</v>
       </c>
-      <c r="N12" s="34"/>
+      <c r="N12" s="43"/>
     </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -29691,7 +29694,7 @@
       <c r="C13" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="43"/>
       <c r="F13" s="1">
         <v>11</v>
       </c>
@@ -29701,7 +29704,7 @@
       <c r="H13" s="24">
         <v>0.48178799999999999</v>
       </c>
-      <c r="I13" s="34"/>
+      <c r="I13" s="43"/>
       <c r="K13" s="1">
         <v>11</v>
       </c>
@@ -29711,9 +29714,9 @@
       <c r="M13" s="24">
         <v>0.52152299999999996</v>
       </c>
-      <c r="N13" s="34"/>
+      <c r="N13" s="43"/>
     </row>
-    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -29723,7 +29726,7 @@
       <c r="C14" s="24">
         <v>0.47516599999999998</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="43"/>
       <c r="F14" s="1">
         <v>12</v>
       </c>
@@ -29733,7 +29736,7 @@
       <c r="H14" s="24">
         <v>0.48675499999999999</v>
       </c>
-      <c r="I14" s="34"/>
+      <c r="I14" s="43"/>
       <c r="K14" s="1">
         <v>12</v>
       </c>
@@ -29743,7 +29746,7 @@
       <c r="M14" s="24">
         <v>0.50331099999999995</v>
       </c>
-      <c r="N14" s="34"/>
+      <c r="N14" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -29764,9 +29767,9 @@
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -29795,7 +29798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -29805,7 +29808,7 @@
       <c r="C2" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="43" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="1">
@@ -29817,7 +29820,7 @@
       <c r="H2" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="43" t="s">
         <v>25</v>
       </c>
       <c r="K2" s="1">
@@ -29829,11 +29832,11 @@
       <c r="M2" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -29843,7 +29846,7 @@
       <c r="C3" s="24">
         <v>0.569546</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="43"/>
       <c r="F3" s="1">
         <v>1</v>
       </c>
@@ -29853,7 +29856,7 @@
       <c r="H3" s="24">
         <v>0.56991199999999997</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="43"/>
       <c r="K3" s="1">
         <v>1</v>
       </c>
@@ -29863,9 +29866,9 @@
       <c r="M3" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="N3" s="34"/>
+      <c r="N3" s="43"/>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -29875,7 +29878,7 @@
       <c r="C4" s="24">
         <v>0.567716</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="43"/>
       <c r="F4" s="1">
         <v>2</v>
       </c>
@@ -29885,7 +29888,7 @@
       <c r="H4" s="24">
         <v>0.56881400000000004</v>
       </c>
-      <c r="I4" s="34"/>
+      <c r="I4" s="43"/>
       <c r="K4" s="1">
         <v>2</v>
       </c>
@@ -29895,9 +29898,9 @@
       <c r="M4" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="N4" s="34"/>
+      <c r="N4" s="43"/>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -29907,7 +29910,7 @@
       <c r="C5" s="24">
         <v>0.58894599999999997</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="43"/>
       <c r="F5" s="1">
         <v>3</v>
       </c>
@@ -29917,7 +29920,7 @@
       <c r="H5" s="24">
         <v>0.58308899999999997</v>
       </c>
-      <c r="I5" s="34"/>
+      <c r="I5" s="43"/>
       <c r="K5" s="1">
         <v>3</v>
       </c>
@@ -29927,9 +29930,9 @@
       <c r="M5" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="N5" s="34"/>
+      <c r="N5" s="43"/>
     </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -29939,7 +29942,7 @@
       <c r="C6" s="24">
         <v>0.60175699999999999</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="43"/>
       <c r="F6" s="1">
         <v>4</v>
       </c>
@@ -29949,7 +29952,7 @@
       <c r="H6" s="24">
         <v>0.60651500000000003</v>
       </c>
-      <c r="I6" s="34"/>
+      <c r="I6" s="43"/>
       <c r="K6" s="1">
         <v>4</v>
       </c>
@@ -29959,9 +29962,9 @@
       <c r="M6" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="N6" s="34"/>
+      <c r="N6" s="43"/>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -29971,7 +29974,7 @@
       <c r="C7" s="24">
         <v>0.61712999999999996</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="43"/>
       <c r="F7" s="1">
         <v>5</v>
       </c>
@@ -29981,7 +29984,7 @@
       <c r="H7" s="24">
         <v>0.61786200000000002</v>
       </c>
-      <c r="I7" s="34"/>
+      <c r="I7" s="43"/>
       <c r="K7" s="1">
         <v>5</v>
       </c>
@@ -29991,9 +29994,9 @@
       <c r="M7" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="N7" s="34"/>
+      <c r="N7" s="43"/>
     </row>
-    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -30003,7 +30006,7 @@
       <c r="C8" s="24">
         <v>0.620425</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="43"/>
       <c r="F8" s="1">
         <v>6</v>
       </c>
@@ -30013,7 +30016,7 @@
       <c r="H8" s="24">
         <v>0.61090800000000001</v>
       </c>
-      <c r="I8" s="34"/>
+      <c r="I8" s="43"/>
       <c r="K8" s="1">
         <v>6</v>
       </c>
@@ -30023,9 +30026,9 @@
       <c r="M8" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="N8" s="34"/>
+      <c r="N8" s="43"/>
     </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -30035,7 +30038,7 @@
       <c r="C9" s="24">
         <v>0.633602</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="43"/>
       <c r="F9" s="1">
         <v>7</v>
       </c>
@@ -30045,7 +30048,7 @@
       <c r="H9" s="24">
         <v>0.61786200000000002</v>
       </c>
-      <c r="I9" s="34"/>
+      <c r="I9" s="43"/>
       <c r="K9" s="1">
         <v>7</v>
       </c>
@@ -30055,9 +30058,9 @@
       <c r="M9" s="24">
         <v>0.56552000000000002</v>
       </c>
-      <c r="N9" s="34"/>
+      <c r="N9" s="43"/>
     </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -30067,7 +30070,7 @@
       <c r="C10" s="24">
         <v>0.62847699999999995</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="43"/>
       <c r="F10" s="1">
         <v>8</v>
       </c>
@@ -30077,7 +30080,7 @@
       <c r="H10" s="24">
         <v>0.620425</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="43"/>
       <c r="K10" s="1">
         <v>8</v>
       </c>
@@ -30087,9 +30090,9 @@
       <c r="M10" s="24">
         <v>0.57906299999999999</v>
       </c>
-      <c r="N10" s="34"/>
+      <c r="N10" s="43"/>
     </row>
-    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -30099,7 +30102,7 @@
       <c r="C11" s="24">
         <v>0.62664699999999995</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="43"/>
       <c r="F11" s="1">
         <v>9</v>
       </c>
@@ -30109,7 +30112,7 @@
       <c r="H11" s="24">
         <v>0.61712999999999996</v>
       </c>
-      <c r="I11" s="34"/>
+      <c r="I11" s="43"/>
       <c r="K11" s="1">
         <v>9</v>
       </c>
@@ -30119,9 +30122,9 @@
       <c r="M11" s="24">
         <v>0.58491899999999997</v>
       </c>
-      <c r="N11" s="34"/>
+      <c r="N11" s="43"/>
     </row>
-    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -30131,7 +30134,7 @@
       <c r="C12" s="24">
         <v>0.63250399999999996</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="43"/>
       <c r="F12" s="1">
         <v>10</v>
       </c>
@@ -30141,7 +30144,7 @@
       <c r="H12" s="24">
         <v>0.62005900000000003</v>
       </c>
-      <c r="I12" s="34"/>
+      <c r="I12" s="43"/>
       <c r="K12" s="1">
         <v>10</v>
       </c>
@@ -30151,9 +30154,9 @@
       <c r="M12" s="24">
         <v>0.59553400000000001</v>
       </c>
-      <c r="N12" s="34"/>
+      <c r="N12" s="43"/>
     </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -30163,7 +30166,7 @@
       <c r="C13" s="24">
         <v>0.63689600000000002</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="43"/>
       <c r="F13" s="1">
         <v>11</v>
       </c>
@@ -30173,7 +30176,7 @@
       <c r="H13" s="24">
         <v>0.62884300000000004</v>
       </c>
-      <c r="I13" s="34"/>
+      <c r="I13" s="43"/>
       <c r="K13" s="1">
         <v>11</v>
       </c>
@@ -30183,9 +30186,9 @@
       <c r="M13" s="24">
         <v>0.64055600000000001</v>
       </c>
-      <c r="N13" s="34"/>
+      <c r="N13" s="43"/>
     </row>
-    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -30195,7 +30198,7 @@
       <c r="C14" s="24">
         <v>0.64019000000000004</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="43"/>
       <c r="F14" s="1">
         <v>12</v>
       </c>
@@ -30205,7 +30208,7 @@
       <c r="H14" s="24">
         <v>0.63872600000000002</v>
       </c>
-      <c r="I14" s="34"/>
+      <c r="I14" s="43"/>
       <c r="K14" s="1">
         <v>12</v>
       </c>
@@ -30215,7 +30218,7 @@
       <c r="M14" s="24">
         <v>0.66800899999999996</v>
       </c>
-      <c r="N14" s="34"/>
+      <c r="N14" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
type: feat Save the layerwise graphs for defdetection
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/detailed_results.xlsx
+++ b/POS Code/Experiments/attachments/detailed_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91492F5E-7C69-AC45-8D0D-FB3C423E1942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C0DFE6-C94F-6B40-B4DF-4C565AAE6BCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20620" activeTab="6" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="61">
   <si>
     <t>Selection</t>
   </si>
@@ -12219,6 +12219,1018 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="465157695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DefDectLayerwise!$L$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DefDectLayerwise!$K$61:$K$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DefDectLayerwise!$L$61:$L$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56076099999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57430499999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58162499999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.58565199999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57796499999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57357199999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57686700000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.577233</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57686700000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57430499999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.57613499999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.57576899999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-201A-B14F-B7D4-6A9AD25B059A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DefDectLayerwise!$M$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incremental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DefDectLayerwise!$K$61:$K$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DefDectLayerwise!$M$61:$M$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56698400000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57430499999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57979499999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.571376</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57906299999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57210799999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56625199999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57650100000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57503700000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57467100000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56625199999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.57284000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-201A-B14F-B7D4-6A9AD25B059A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1204187680"/>
+        <c:axId val="83206463"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1204187680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="83206463"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="83206463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1204187680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DefDectLayerwise!$B$89</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Independent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DefDectLayerwise!$A$90:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DefDectLayerwise!$B$90:$B$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57101000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56442199999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57101000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57869700000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.569546</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.567716</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56515400000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9EEF-CA43-ABC4-D58202FDEC34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DefDectLayerwise!$C$89</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incremental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DefDectLayerwise!$A$90:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DefDectLayerwise!$C$90:$C$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56552000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56698400000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.565886</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.569546</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57284000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.51281100000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.51207899999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52562200000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.488653</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.48243000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.48169800000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.48389500000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9EEF-CA43-ABC4-D58202FDEC34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1204987088"/>
+        <c:axId val="1206023280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1204987088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1206023280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1206023280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1204987088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16493,6 +17505,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors30.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors31.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -27800,6 +28892,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style30.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style31.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -32381,6 +34479,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>844550</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1416050</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC3A0AF9-F15A-434A-A61C-9AA495146414}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D4FEC34-FE86-5F4D-B829-F01CE62801CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -35822,7 +37992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F291A794-F81B-A94A-B246-9FC1326ED183}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -39112,10 +41282,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586CC5E8-52EF-824B-9F99-84A3E832E106}">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="K100" sqref="K100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40026,7 +42196,7 @@
       </c>
       <c r="N44" s="47"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="42" t="s">
         <v>33</v>
       </c>
@@ -40045,8 +42215,17 @@
       <c r="H60" s="42" t="s">
         <v>32</v>
       </c>
+      <c r="K60" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="L60" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="M60" s="42" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A61" s="42">
         <v>0</v>
       </c>
@@ -40071,8 +42250,20 @@
       <c r="I61" s="47" t="s">
         <v>60</v>
       </c>
+      <c r="K61" s="42">
+        <v>0</v>
+      </c>
+      <c r="L61" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="M61" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="N61" s="47" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A62" s="42">
         <v>1</v>
       </c>
@@ -40093,8 +42284,18 @@
         <v>0.56295799999999996</v>
       </c>
       <c r="I62" s="47"/>
+      <c r="K62" s="42">
+        <v>1</v>
+      </c>
+      <c r="L62" s="24">
+        <v>0.56076099999999995</v>
+      </c>
+      <c r="M62" s="24">
+        <v>0.56698400000000004</v>
+      </c>
+      <c r="N62" s="47"/>
     </row>
-    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A63" s="42">
         <v>2</v>
       </c>
@@ -40115,8 +42316,18 @@
         <v>0.52928299999999995</v>
       </c>
       <c r="I63" s="47"/>
+      <c r="K63" s="42">
+        <v>2</v>
+      </c>
+      <c r="L63" s="24">
+        <v>0.57430499999999995</v>
+      </c>
+      <c r="M63" s="24">
+        <v>0.57430499999999995</v>
+      </c>
+      <c r="N63" s="47"/>
     </row>
-    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A64" s="42">
         <v>3</v>
       </c>
@@ -40137,8 +42348,18 @@
         <v>0.54904799999999998</v>
       </c>
       <c r="I64" s="47"/>
+      <c r="K64" s="42">
+        <v>3</v>
+      </c>
+      <c r="L64" s="24">
+        <v>0.58162499999999995</v>
+      </c>
+      <c r="M64" s="24">
+        <v>0.57979499999999995</v>
+      </c>
+      <c r="N64" s="47"/>
     </row>
-    <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A65" s="42">
         <v>4</v>
       </c>
@@ -40159,8 +42380,18 @@
         <v>0.52964900000000004</v>
       </c>
       <c r="I65" s="47"/>
+      <c r="K65" s="42">
+        <v>4</v>
+      </c>
+      <c r="L65" s="24">
+        <v>0.58565199999999995</v>
+      </c>
+      <c r="M65" s="24">
+        <v>0.571376</v>
+      </c>
+      <c r="N65" s="47"/>
     </row>
-    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A66" s="42">
         <v>5</v>
       </c>
@@ -40181,8 +42412,18 @@
         <v>0.46559299999999998</v>
       </c>
       <c r="I66" s="47"/>
+      <c r="K66" s="42">
+        <v>5</v>
+      </c>
+      <c r="L66" s="24">
+        <v>0.57796499999999995</v>
+      </c>
+      <c r="M66" s="24">
+        <v>0.57906299999999999</v>
+      </c>
+      <c r="N66" s="47"/>
     </row>
-    <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A67" s="42">
         <v>6</v>
       </c>
@@ -40203,8 +42444,18 @@
         <v>0.58821400000000001</v>
       </c>
       <c r="I67" s="47"/>
+      <c r="K67" s="42">
+        <v>6</v>
+      </c>
+      <c r="L67" s="24">
+        <v>0.57357199999999997</v>
+      </c>
+      <c r="M67" s="24">
+        <v>0.57210799999999995</v>
+      </c>
+      <c r="N67" s="47"/>
     </row>
-    <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A68" s="42">
         <v>7</v>
       </c>
@@ -40225,8 +42476,18 @@
         <v>0.58857999999999999</v>
       </c>
       <c r="I68" s="47"/>
+      <c r="K68" s="42">
+        <v>7</v>
+      </c>
+      <c r="L68" s="24">
+        <v>0.57686700000000002</v>
+      </c>
+      <c r="M68" s="24">
+        <v>0.56625199999999998</v>
+      </c>
+      <c r="N68" s="47"/>
     </row>
-    <row r="69" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A69" s="42">
         <v>8</v>
       </c>
@@ -40247,8 +42508,18 @@
         <v>0.61420200000000003</v>
       </c>
       <c r="I69" s="47"/>
+      <c r="K69" s="42">
+        <v>8</v>
+      </c>
+      <c r="L69" s="24">
+        <v>0.577233</v>
+      </c>
+      <c r="M69" s="24">
+        <v>0.57650100000000004</v>
+      </c>
+      <c r="N69" s="47"/>
     </row>
-    <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A70" s="42">
         <v>9</v>
       </c>
@@ -40269,8 +42540,18 @@
         <v>0.60614900000000005</v>
       </c>
       <c r="I70" s="47"/>
+      <c r="K70" s="42">
+        <v>9</v>
+      </c>
+      <c r="L70" s="24">
+        <v>0.57686700000000002</v>
+      </c>
+      <c r="M70" s="24">
+        <v>0.57503700000000002</v>
+      </c>
+      <c r="N70" s="47"/>
     </row>
-    <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A71" s="42">
         <v>10</v>
       </c>
@@ -40291,8 +42572,18 @@
         <v>0.61603200000000002</v>
       </c>
       <c r="I71" s="47"/>
+      <c r="K71" s="42">
+        <v>10</v>
+      </c>
+      <c r="L71" s="24">
+        <v>0.57430499999999995</v>
+      </c>
+      <c r="M71" s="24">
+        <v>0.57467100000000004</v>
+      </c>
+      <c r="N71" s="47"/>
     </row>
-    <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A72" s="42">
         <v>11</v>
       </c>
@@ -40313,8 +42604,18 @@
         <v>0.59919500000000003</v>
       </c>
       <c r="I72" s="47"/>
+      <c r="K72" s="42">
+        <v>11</v>
+      </c>
+      <c r="L72" s="24">
+        <v>0.57613499999999995</v>
+      </c>
+      <c r="M72" s="24">
+        <v>0.56625199999999998</v>
+      </c>
+      <c r="N72" s="47"/>
     </row>
-    <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="16" x14ac:dyDescent="0.25">
       <c r="A73" s="42">
         <v>12</v>
       </c>
@@ -40335,11 +42636,192 @@
         <v>0.59260599999999997</v>
       </c>
       <c r="I73" s="47"/>
+      <c r="K73" s="42">
+        <v>12</v>
+      </c>
+      <c r="L73" s="24">
+        <v>0.57576899999999998</v>
+      </c>
+      <c r="M73" s="24">
+        <v>0.57284000000000002</v>
+      </c>
+      <c r="N73" s="47"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B89" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C89" s="42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A90" s="42">
+        <v>0</v>
+      </c>
+      <c r="B90" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="C90" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="D90" s="47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A91" s="42">
+        <v>1</v>
+      </c>
+      <c r="B91" s="24">
+        <v>0.57101000000000002</v>
+      </c>
+      <c r="C91" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="D91" s="47"/>
+    </row>
+    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A92" s="42">
+        <v>2</v>
+      </c>
+      <c r="B92" s="24">
+        <v>0.56442199999999998</v>
+      </c>
+      <c r="C92" s="24">
+        <v>0.56698400000000004</v>
+      </c>
+      <c r="D92" s="47"/>
+    </row>
+    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A93" s="42">
+        <v>3</v>
+      </c>
+      <c r="B93" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="C93" s="24">
+        <v>0.565886</v>
+      </c>
+      <c r="D93" s="47"/>
+    </row>
+    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A94" s="42">
+        <v>4</v>
+      </c>
+      <c r="B94" s="24">
+        <v>0.57101000000000002</v>
+      </c>
+      <c r="C94" s="24">
+        <v>0.569546</v>
+      </c>
+      <c r="D94" s="47"/>
+    </row>
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A95" s="42">
+        <v>5</v>
+      </c>
+      <c r="B95" s="24">
+        <v>0.57869700000000002</v>
+      </c>
+      <c r="C95" s="24">
+        <v>0.57284000000000002</v>
+      </c>
+      <c r="D95" s="47"/>
+    </row>
+    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A96" s="42">
+        <v>6</v>
+      </c>
+      <c r="B96" s="24">
+        <v>0.569546</v>
+      </c>
+      <c r="C96" s="24">
+        <v>0.51281100000000002</v>
+      </c>
+      <c r="D96" s="47"/>
+    </row>
+    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A97" s="42">
+        <v>7</v>
+      </c>
+      <c r="B97" s="24">
+        <v>0.567716</v>
+      </c>
+      <c r="C97" s="24">
+        <v>0.51207899999999995</v>
+      </c>
+      <c r="D97" s="47"/>
+    </row>
+    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A98" s="42">
+        <v>8</v>
+      </c>
+      <c r="B98" s="24">
+        <v>0.56515400000000005</v>
+      </c>
+      <c r="C98" s="24">
+        <v>0.52562200000000003</v>
+      </c>
+      <c r="D98" s="47"/>
+    </row>
+    <row r="99" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A99" s="42">
+        <v>9</v>
+      </c>
+      <c r="B99" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="C99" s="24">
+        <v>0.488653</v>
+      </c>
+      <c r="D99" s="47"/>
+    </row>
+    <row r="100" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A100" s="42">
+        <v>10</v>
+      </c>
+      <c r="B100" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="C100" s="24">
+        <v>0.48243000000000003</v>
+      </c>
+      <c r="D100" s="47"/>
+    </row>
+    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A101" s="42">
+        <v>11</v>
+      </c>
+      <c r="B101" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="C101" s="24">
+        <v>0.48169800000000002</v>
+      </c>
+      <c r="D101" s="47"/>
+    </row>
+    <row r="102" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A102" s="42">
+        <v>12</v>
+      </c>
+      <c r="B102" s="24">
+        <v>0.56552000000000002</v>
+      </c>
+      <c r="C102" s="24">
+        <v>0.48389500000000002</v>
+      </c>
+      <c r="D102" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="D61:D73"/>
     <mergeCell ref="I61:I73"/>
+    <mergeCell ref="N61:N73"/>
+    <mergeCell ref="D90:D102"/>
     <mergeCell ref="D2:D14"/>
     <mergeCell ref="I2:I14"/>
     <mergeCell ref="N2:N14"/>

</xml_diff>